<commit_message>
Rearrange processing order and cleanup
</commit_message>
<xml_diff>
--- a/reports/zonal_distribution_resident_passengers.xlsx
+++ b/reports/zonal_distribution_resident_passengers.xlsx
@@ -478,22 +478,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C2" t="n">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="D2" t="n">
-        <v>292.4885902952402</v>
+        <v>153</v>
       </c>
       <c r="E2" t="n">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="F2" t="n">
-        <v>203</v>
+        <v>229</v>
       </c>
       <c r="G2" t="n">
-        <v>526.8441995187937</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3">
@@ -503,22 +503,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C3" t="n">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="D3" t="n">
-        <v>711.3347177625194</v>
+        <v>208</v>
       </c>
       <c r="E3" t="n">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="F3" t="n">
-        <v>370</v>
+        <v>391</v>
       </c>
       <c r="G3" t="n">
-        <v>2361.19136066915</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4">
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D4" t="n">
-        <v>93.64261768814296</v>
+        <v>40</v>
       </c>
       <c r="E4" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G4" t="n">
-        <v>213.0965688625636</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
@@ -553,22 +553,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
+        <v>27</v>
+      </c>
+      <c r="D5" t="n">
         <v>26</v>
       </c>
-      <c r="D5" t="n">
-        <v>51.84697728809346</v>
-      </c>
       <c r="E5" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="n">
+        <v>37</v>
+      </c>
+      <c r="G5" t="n">
         <v>36</v>
-      </c>
-      <c r="G5" t="n">
-        <v>86.78637822663244</v>
       </c>
     </row>
     <row r="6">
@@ -578,22 +578,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D6" t="n">
-        <v>194.9733874890915</v>
+        <v>77</v>
       </c>
       <c r="E6" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F6" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G6" t="n">
-        <v>420.0230771500916</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7">
@@ -603,22 +603,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C7" t="n">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D7" t="n">
-        <v>172.1939130706724</v>
+        <v>85</v>
       </c>
       <c r="E7" t="n">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F7" t="n">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="G7" t="n">
-        <v>374.6553754313406</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
@@ -628,22 +628,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C8" t="n">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D8" t="n">
-        <v>338.4956636218766</v>
+        <v>90</v>
       </c>
       <c r="E8" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F8" t="n">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="G8" t="n">
-        <v>1177.077347882569</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9">
@@ -659,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="D9" t="n">
-        <v>28.3366914739767</v>
+        <v>16</v>
       </c>
       <c r="E9" t="n">
         <v>10</v>
@@ -668,7 +668,7 @@
         <v>20</v>
       </c>
       <c r="G9" t="n">
-        <v>38.01188183469321</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -678,22 +678,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C10" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D10" t="n">
-        <v>116.5590052697882</v>
+        <v>66</v>
       </c>
       <c r="E10" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F10" t="n">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G10" t="n">
-        <v>171.6480161049426</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11">
@@ -709,7 +709,7 @@
         <v>14</v>
       </c>
       <c r="D11" t="n">
-        <v>35.24575250742617</v>
+        <v>14</v>
       </c>
       <c r="E11" t="n">
         <v>11</v>
@@ -718,7 +718,7 @@
         <v>22</v>
       </c>
       <c r="G11" t="n">
-        <v>63.00802359259052</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -734,7 +734,7 @@
         <v>33</v>
       </c>
       <c r="D12" t="n">
-        <v>141.7173131862031</v>
+        <v>33</v>
       </c>
       <c r="E12" t="n">
         <v>35</v>
@@ -743,7 +743,7 @@
         <v>69</v>
       </c>
       <c r="G12" t="n">
-        <v>681.7801362904765</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13">
@@ -753,22 +753,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C13" t="n">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="D13" t="n">
-        <v>292.8424057954805</v>
+        <v>135</v>
       </c>
       <c r="E13" t="n">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F13" t="n">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="G13" t="n">
-        <v>593.5761476797395</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14">
@@ -778,22 +778,22 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D14" t="n">
-        <v>108.4315070116118</v>
+        <v>51</v>
       </c>
       <c r="E14" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F14" t="n">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G14" t="n">
-        <v>188.6821424217474</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15">
@@ -803,22 +803,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="C15" t="n">
-        <v>239</v>
+        <v>274</v>
       </c>
       <c r="D15" t="n">
-        <v>699.9445421634921</v>
+        <v>269</v>
       </c>
       <c r="E15" t="n">
-        <v>212</v>
+        <v>243</v>
       </c>
       <c r="F15" t="n">
-        <v>422</v>
+        <v>472</v>
       </c>
       <c r="G15" t="n">
-        <v>2043.640348183798</v>
+        <v>463</v>
       </c>
     </row>
     <row r="16">
@@ -828,22 +828,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>797</v>
+        <v>989</v>
       </c>
       <c r="C16" t="n">
-        <v>1576</v>
+        <v>1906</v>
       </c>
       <c r="D16" t="n">
-        <v>4012.763155759468</v>
+        <v>1836</v>
       </c>
       <c r="E16" t="n">
-        <v>1244</v>
+        <v>1570</v>
       </c>
       <c r="F16" t="n">
-        <v>2465</v>
+        <v>3016</v>
       </c>
       <c r="G16" t="n">
-        <v>9828.473771308905</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="17">
@@ -853,22 +853,22 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" t="n">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D17" t="n">
-        <v>164.8364240895055</v>
+        <v>58</v>
       </c>
       <c r="E17" t="n">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F17" t="n">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="G17" t="n">
-        <v>527.4339953915301</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18">
@@ -878,22 +878,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18" t="n">
+        <v>19</v>
+      </c>
+      <c r="D18" t="n">
         <v>18</v>
       </c>
-      <c r="D18" t="n">
-        <v>43.98416920614759</v>
-      </c>
       <c r="E18" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F18" t="n">
+        <v>27</v>
+      </c>
+      <c r="G18" t="n">
         <v>26</v>
-      </c>
-      <c r="G18" t="n">
-        <v>84.95431503120587</v>
       </c>
     </row>
     <row r="19">
@@ -909,7 +909,7 @@
         <v>12</v>
       </c>
       <c r="D19" t="n">
-        <v>27.73569131627352</v>
+        <v>12</v>
       </c>
       <c r="E19" t="n">
         <v>9</v>
@@ -918,7 +918,7 @@
         <v>18</v>
       </c>
       <c r="G19" t="n">
-        <v>45.28465470270577</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
@@ -928,22 +928,22 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D20" t="n">
-        <v>64.61316482390929</v>
+        <v>26</v>
       </c>
       <c r="E20" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F20" t="n">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G20" t="n">
-        <v>171.8938651302715</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21">
@@ -953,22 +953,22 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C21" t="n">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="D21" t="n">
-        <v>1038.556966747412</v>
+        <v>254</v>
       </c>
       <c r="E21" t="n">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="F21" t="n">
-        <v>608</v>
+        <v>591</v>
       </c>
       <c r="G21" t="n">
-        <v>3668.026532723073</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -1032,22 +1032,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C2" t="n">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="D2" t="n">
-        <v>428.0549411780708</v>
+        <v>146</v>
       </c>
       <c r="E2" t="n">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="F2" t="n">
-        <v>210</v>
+        <v>257</v>
       </c>
       <c r="G2" t="n">
-        <v>1427.068212755847</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3">
@@ -1055,22 +1055,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>350</v>
+        <v>442</v>
       </c>
       <c r="C3" t="n">
-        <v>689</v>
+        <v>846</v>
       </c>
       <c r="D3" t="n">
-        <v>1814.357443196731</v>
+        <v>805</v>
       </c>
       <c r="E3" t="n">
-        <v>565</v>
+        <v>711</v>
       </c>
       <c r="F3" t="n">
-        <v>1116</v>
+        <v>1361</v>
       </c>
       <c r="G3" t="n">
-        <v>4579.221813028876</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="4">
@@ -1078,22 +1078,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>444</v>
+        <v>528</v>
       </c>
       <c r="C4" t="n">
-        <v>879</v>
+        <v>1028</v>
       </c>
       <c r="D4" t="n">
-        <v>2133.674078262204</v>
+        <v>1006</v>
       </c>
       <c r="E4" t="n">
-        <v>685</v>
+        <v>838</v>
       </c>
       <c r="F4" t="n">
-        <v>1359</v>
+        <v>1629</v>
       </c>
       <c r="G4" t="n">
-        <v>5010.17304689853</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="5">
@@ -1101,22 +1101,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C5" t="n">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="D5" t="n">
-        <v>816.7752897589887</v>
+        <v>267</v>
       </c>
       <c r="E5" t="n">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="F5" t="n">
-        <v>442</v>
+        <v>469</v>
       </c>
       <c r="G5" t="n">
-        <v>2512.470793619224</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6">
@@ -1124,22 +1124,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="C6" t="n">
-        <v>292</v>
+        <v>321</v>
       </c>
       <c r="D6" t="n">
-        <v>767.6735760273507</v>
+        <v>317</v>
       </c>
       <c r="E6" t="n">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="F6" t="n">
-        <v>485</v>
+        <v>522</v>
       </c>
       <c r="G6" t="n">
-        <v>1949.73505025599</v>
+        <v>516</v>
       </c>
     </row>
     <row r="7">
@@ -1147,22 +1147,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="C7" t="n">
-        <v>413</v>
+        <v>457</v>
       </c>
       <c r="D7" t="n">
-        <v>900.9134211179203</v>
+        <v>450</v>
       </c>
       <c r="E7" t="n">
-        <v>294</v>
+        <v>334</v>
       </c>
       <c r="F7" t="n">
-        <v>581</v>
+        <v>658</v>
       </c>
       <c r="G7" t="n">
-        <v>1756.762086194048</v>
+        <v>649</v>
       </c>
     </row>
     <row r="8">
@@ -1170,22 +1170,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C8" t="n">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="D8" t="n">
-        <v>704.702734615641</v>
+        <v>214</v>
       </c>
       <c r="E8" t="n">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="F8" t="n">
-        <v>378</v>
+        <v>402</v>
       </c>
       <c r="G8" t="n">
-        <v>2305.501441534878</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9">
@@ -1199,7 +1199,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>25.83420566201216</v>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
         <v>6</v>
@@ -1208,7 +1208,7 @@
         <v>12</v>
       </c>
       <c r="G9" t="n">
-        <v>57.12916112635393</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -1216,22 +1216,22 @@
         <v>99</v>
       </c>
       <c r="B10" t="n">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C10" t="n">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="D10" t="n">
-        <v>1038.556966747412</v>
+        <v>254</v>
       </c>
       <c r="E10" t="n">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="F10" t="n">
-        <v>608</v>
+        <v>591</v>
       </c>
       <c r="G10" t="n">
-        <v>3668.026532723073</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduce pii, introduce additional data processing, impute missing respondents, calc unchosen alternatives trip characteristics
alters notebook file structure to separate data processing and EDA notebooks
</commit_message>
<xml_diff>
--- a/reports/zonal_distribution_resident_passengers.xlsx
+++ b/reports/zonal_distribution_resident_passengers.xlsx
@@ -484,7 +484,7 @@
         <v>155</v>
       </c>
       <c r="D2" t="n">
-        <v>153</v>
+        <v>155.3578315248243</v>
       </c>
       <c r="E2" t="n">
         <v>115</v>
@@ -493,7 +493,7 @@
         <v>229</v>
       </c>
       <c r="G2" t="n">
-        <v>227</v>
+        <v>260.5158083523038</v>
       </c>
     </row>
     <row r="3">
@@ -509,7 +509,7 @@
         <v>214</v>
       </c>
       <c r="D3" t="n">
-        <v>208</v>
+        <v>279.4997003628848</v>
       </c>
       <c r="E3" t="n">
         <v>201</v>
@@ -518,7 +518,7 @@
         <v>391</v>
       </c>
       <c r="G3" t="n">
-        <v>380</v>
+        <v>785.6449465616154</v>
       </c>
     </row>
     <row r="4">
@@ -534,7 +534,7 @@
         <v>40</v>
       </c>
       <c r="D4" t="n">
-        <v>40</v>
+        <v>46.47836900713188</v>
       </c>
       <c r="E4" t="n">
         <v>33</v>
@@ -543,7 +543,7 @@
         <v>66</v>
       </c>
       <c r="G4" t="n">
-        <v>66</v>
+        <v>91.87176664801527</v>
       </c>
     </row>
     <row r="5">
@@ -559,7 +559,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="n">
-        <v>26</v>
+        <v>27.12191921329827</v>
       </c>
       <c r="E5" t="n">
         <v>19</v>
@@ -568,7 +568,7 @@
         <v>37</v>
       </c>
       <c r="G5" t="n">
-        <v>36</v>
+        <v>42.34514907366468</v>
       </c>
     </row>
     <row r="6">
@@ -584,7 +584,7 @@
         <v>77</v>
       </c>
       <c r="D6" t="n">
-        <v>77</v>
+        <v>90.32100206688119</v>
       </c>
       <c r="E6" t="n">
         <v>71</v>
@@ -593,7 +593,7 @@
         <v>137</v>
       </c>
       <c r="G6" t="n">
-        <v>137</v>
+        <v>181.0218630137317</v>
       </c>
     </row>
     <row r="7">
@@ -609,7 +609,7 @@
         <v>89</v>
       </c>
       <c r="D7" t="n">
-        <v>85</v>
+        <v>88.83820760501696</v>
       </c>
       <c r="E7" t="n">
         <v>63</v>
@@ -618,7 +618,7 @@
         <v>124</v>
       </c>
       <c r="G7" t="n">
-        <v>118</v>
+        <v>156.0973323957411</v>
       </c>
     </row>
     <row r="8">
@@ -634,7 +634,7 @@
         <v>92</v>
       </c>
       <c r="D8" t="n">
-        <v>90</v>
+        <v>124.0634955533343</v>
       </c>
       <c r="E8" t="n">
         <v>83</v>
@@ -643,7 +643,7 @@
         <v>166</v>
       </c>
       <c r="G8" t="n">
-        <v>164</v>
+        <v>330.4634125965265</v>
       </c>
     </row>
     <row r="9">
@@ -659,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="D9" t="n">
-        <v>16</v>
+        <v>15.53705587946277</v>
       </c>
       <c r="E9" t="n">
         <v>10</v>
@@ -668,7 +668,7 @@
         <v>20</v>
       </c>
       <c r="G9" t="n">
-        <v>20</v>
+        <v>20.32971258737049</v>
       </c>
     </row>
     <row r="10">
@@ -684,7 +684,7 @@
         <v>66</v>
       </c>
       <c r="D10" t="n">
-        <v>66</v>
+        <v>61.06399030587847</v>
       </c>
       <c r="E10" t="n">
         <v>46</v>
@@ -693,7 +693,7 @@
         <v>87</v>
       </c>
       <c r="G10" t="n">
-        <v>87</v>
+        <v>81.53694608399567</v>
       </c>
     </row>
     <row r="11">
@@ -709,7 +709,7 @@
         <v>14</v>
       </c>
       <c r="D11" t="n">
-        <v>14</v>
+        <v>17.23362346163252</v>
       </c>
       <c r="E11" t="n">
         <v>11</v>
@@ -718,7 +718,7 @@
         <v>22</v>
       </c>
       <c r="G11" t="n">
-        <v>22</v>
+        <v>29.29661505819229</v>
       </c>
     </row>
     <row r="12">
@@ -734,7 +734,7 @@
         <v>33</v>
       </c>
       <c r="D12" t="n">
-        <v>33</v>
+        <v>50.11702191503642</v>
       </c>
       <c r="E12" t="n">
         <v>35</v>
@@ -743,7 +743,7 @@
         <v>69</v>
       </c>
       <c r="G12" t="n">
-        <v>69</v>
+        <v>186.6480070359511</v>
       </c>
     </row>
     <row r="13">
@@ -759,7 +759,7 @@
         <v>135</v>
       </c>
       <c r="D13" t="n">
-        <v>135</v>
+        <v>137.8518712211186</v>
       </c>
       <c r="E13" t="n">
         <v>95</v>
@@ -768,7 +768,7 @@
         <v>186</v>
       </c>
       <c r="G13" t="n">
-        <v>186</v>
+        <v>231.6849390244221</v>
       </c>
     </row>
     <row r="14">
@@ -784,7 +784,7 @@
         <v>53</v>
       </c>
       <c r="D14" t="n">
-        <v>51</v>
+        <v>56.1836652679048</v>
       </c>
       <c r="E14" t="n">
         <v>42</v>
@@ -793,7 +793,7 @@
         <v>83</v>
       </c>
       <c r="G14" t="n">
-        <v>77</v>
+        <v>93.91208427609222</v>
       </c>
     </row>
     <row r="15">
@@ -809,7 +809,7 @@
         <v>274</v>
       </c>
       <c r="D15" t="n">
-        <v>269</v>
+        <v>320.6245116209929</v>
       </c>
       <c r="E15" t="n">
         <v>243</v>
@@ -818,7 +818,7 @@
         <v>472</v>
       </c>
       <c r="G15" t="n">
-        <v>463</v>
+        <v>742.7761373426529</v>
       </c>
     </row>
     <row r="16">
@@ -834,7 +834,7 @@
         <v>1906</v>
       </c>
       <c r="D16" t="n">
-        <v>1836</v>
+        <v>2095.768818718121</v>
       </c>
       <c r="E16" t="n">
         <v>1570</v>
@@ -843,7 +843,7 @@
         <v>3016</v>
       </c>
       <c r="G16" t="n">
-        <v>2899</v>
+        <v>4389.007663717412</v>
       </c>
     </row>
     <row r="17">
@@ -859,7 +859,7 @@
         <v>58</v>
       </c>
       <c r="D17" t="n">
-        <v>58</v>
+        <v>75.49698962654575</v>
       </c>
       <c r="E17" t="n">
         <v>52</v>
@@ -868,7 +868,7 @@
         <v>104</v>
       </c>
       <c r="G17" t="n">
-        <v>104</v>
+        <v>190.9434917195673</v>
       </c>
     </row>
     <row r="18">
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="D18" t="n">
-        <v>18</v>
+        <v>20.35745769377773</v>
       </c>
       <c r="E18" t="n">
         <v>14</v>
@@ -893,7 +893,7 @@
         <v>27</v>
       </c>
       <c r="G18" t="n">
-        <v>26</v>
+        <v>34.79091803031537</v>
       </c>
     </row>
     <row r="19">
@@ -909,7 +909,7 @@
         <v>12</v>
       </c>
       <c r="D19" t="n">
-        <v>12</v>
+        <v>13.82287693663128</v>
       </c>
       <c r="E19" t="n">
         <v>9</v>
@@ -918,7 +918,7 @@
         <v>18</v>
       </c>
       <c r="G19" t="n">
-        <v>18</v>
+        <v>21.86874613393865</v>
       </c>
     </row>
     <row r="20">
@@ -934,7 +934,7 @@
         <v>26</v>
       </c>
       <c r="D20" t="n">
-        <v>26</v>
+        <v>37.36800264078069</v>
       </c>
       <c r="E20" t="n">
         <v>28</v>
@@ -943,7 +943,7 @@
         <v>56</v>
       </c>
       <c r="G20" t="n">
-        <v>56</v>
+        <v>114.7581598461426</v>
       </c>
     </row>
     <row r="21">
@@ -959,7 +959,7 @@
         <v>293</v>
       </c>
       <c r="D21" t="n">
-        <v>254</v>
+        <v>373.6469898604245</v>
       </c>
       <c r="E21" t="n">
         <v>327</v>
@@ -968,7 +968,7 @@
         <v>591</v>
       </c>
       <c r="G21" t="n">
-        <v>529</v>
+        <v>1247.330569872149</v>
       </c>
     </row>
   </sheetData>
@@ -1038,7 +1038,7 @@
         <v>155</v>
       </c>
       <c r="D2" t="n">
-        <v>146</v>
+        <v>173.83596285659</v>
       </c>
       <c r="E2" t="n">
         <v>135</v>
@@ -1047,7 +1047,7 @@
         <v>257</v>
       </c>
       <c r="G2" t="n">
-        <v>241</v>
+        <v>434.8040794200455</v>
       </c>
     </row>
     <row r="3">
@@ -1061,7 +1061,7 @@
         <v>846</v>
       </c>
       <c r="D3" t="n">
-        <v>805</v>
+        <v>907.8183451033077</v>
       </c>
       <c r="E3" t="n">
         <v>711</v>
@@ -1070,7 +1070,7 @@
         <v>1361</v>
       </c>
       <c r="G3" t="n">
-        <v>1284</v>
+        <v>1858.356790161298</v>
       </c>
     </row>
     <row r="4">
@@ -1084,7 +1084,7 @@
         <v>1028</v>
       </c>
       <c r="D4" t="n">
-        <v>1006</v>
+        <v>1176.797300265687</v>
       </c>
       <c r="E4" t="n">
         <v>838</v>
@@ -1093,7 +1093,7 @@
         <v>1629</v>
       </c>
       <c r="G4" t="n">
-        <v>1600</v>
+        <v>2513.78311302086</v>
       </c>
     </row>
     <row r="5">
@@ -1107,7 +1107,7 @@
         <v>274</v>
       </c>
       <c r="D5" t="n">
-        <v>267</v>
+        <v>332.0095273340321</v>
       </c>
       <c r="E5" t="n">
         <v>243</v>
@@ -1116,7 +1116,7 @@
         <v>469</v>
       </c>
       <c r="G5" t="n">
-        <v>456</v>
+        <v>856.2437450898512</v>
       </c>
     </row>
     <row r="6">
@@ -1130,7 +1130,7 @@
         <v>321</v>
       </c>
       <c r="D6" t="n">
-        <v>317</v>
+        <v>365.7409831235498</v>
       </c>
       <c r="E6" t="n">
         <v>267</v>
@@ -1139,7 +1139,7 @@
         <v>522</v>
       </c>
       <c r="G6" t="n">
-        <v>516</v>
+        <v>756.5429240343315</v>
       </c>
     </row>
     <row r="7">
@@ -1153,7 +1153,7 @@
         <v>457</v>
       </c>
       <c r="D7" t="n">
-        <v>450</v>
+        <v>464.7854455783876</v>
       </c>
       <c r="E7" t="n">
         <v>334</v>
@@ -1162,7 +1162,7 @@
         <v>658</v>
       </c>
       <c r="G7" t="n">
-        <v>649</v>
+        <v>817.4292232033445</v>
       </c>
     </row>
     <row r="8">
@@ -1176,7 +1176,7 @@
         <v>217</v>
       </c>
       <c r="D8" t="n">
-        <v>214</v>
+        <v>281.5214368060617</v>
       </c>
       <c r="E8" t="n">
         <v>206</v>
@@ -1185,7 +1185,7 @@
         <v>402</v>
       </c>
       <c r="G8" t="n">
-        <v>397</v>
+        <v>728.1156113856521</v>
       </c>
     </row>
     <row r="9">
@@ -1199,7 +1199,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>10.59740955363887</v>
       </c>
       <c r="E9" t="n">
         <v>6</v>
@@ -1208,7 +1208,7 @@
         <v>12</v>
       </c>
       <c r="G9" t="n">
-        <v>12</v>
+        <v>20.23821318226879</v>
       </c>
     </row>
     <row r="10">
@@ -1222,7 +1222,7 @@
         <v>293</v>
       </c>
       <c r="D10" t="n">
-        <v>254</v>
+        <v>373.6469898604245</v>
       </c>
       <c r="E10" t="n">
         <v>327</v>
@@ -1231,7 +1231,7 @@
         <v>591</v>
       </c>
       <c r="G10" t="n">
-        <v>529</v>
+        <v>1247.330569872149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>